<commit_message>
simplify nixie daughter board
Remove cathode pins that would not be usable for current sensing anyway.
Pivot to using anode pin as shunt measurement with a R2R flash ADC (not yet implemented).
</commit_message>
<xml_diff>
--- a/KiCad/nixieAccurateClock/boost-convertor-calcs.xlsx
+++ b/KiCad/nixieAccurateClock/boost-convertor-calcs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Nextcloud\Documents\Projects\nixieclock\nixie-clock-ice\KiCad\nixieAccurateClock\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Nextcloud\Documents\Projects\nixieclock\nixie-clock-ice\KiCad\nixieAccurateClock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C5CF23-C05A-4C5A-84F8-6B3107187708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1929C828-BF49-40A9-B433-48AAA483BE00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{4C5F7C1F-78F8-476C-9393-F25C88E783DB}"/>
+    <workbookView xWindow="-25560" yWindow="8310" windowWidth="23010" windowHeight="12360" xr2:uid="{4C5F7C1F-78F8-476C-9393-F25C88E783DB}"/>
   </bookViews>
   <sheets>
     <sheet name="HV supply" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>Calcs from Art of Electronics - 3rd Edition, Section 9.6.6.a Boost convertor equations (continuous-conduction mode)</t>
   </si>
@@ -124,6 +124,27 @@
   </si>
   <si>
     <t>Ohm</t>
+  </si>
+  <si>
+    <t>Vres-max</t>
+  </si>
+  <si>
+    <t>Vres-min</t>
+  </si>
+  <si>
+    <t>Vres-nom</t>
+  </si>
+  <si>
+    <t>Pres-min</t>
+  </si>
+  <si>
+    <t>Pres-nom</t>
+  </si>
+  <si>
+    <t>Pres-max</t>
+  </si>
+  <si>
+    <t>W</t>
   </si>
 </sst>
 </file>
@@ -522,23 +543,23 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.734375" customWidth="1"/>
-    <col min="2" max="2" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>20</v>
       </c>
@@ -549,7 +570,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -569,7 +590,7 @@
         <v>1.6799999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -586,7 +607,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -603,7 +624,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -623,7 +644,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -640,7 +661,7 @@
         <v>8.1999999999999998E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -660,7 +681,7 @@
         <v>1.5999999999999999E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -680,7 +701,7 @@
         <v>5.9523809523809521E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -697,7 +718,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -714,7 +735,7 @@
         <v>0.97619047619047616</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -734,7 +755,7 @@
         <v>7.0861678004535298E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -754,7 +775,7 @@
         <v>0.70559999999999923</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -774,7 +795,7 @@
         <v>0.735361904761904</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -817,13 +838,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC08BD06-1481-42B4-888E-47F007A488BE}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -834,7 +858,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -845,7 +869,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -857,7 +881,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -869,7 +893,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -879,6 +903,78 @@
       </c>
       <c r="C6" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1">
+        <f>B4*B3</f>
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1">
+        <f>B5*B3</f>
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1">
+        <f>B6*B3</f>
+        <v>65</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="1">
+        <f>B4*B8</f>
+        <v>7.5757575757575758E-4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="1">
+        <f>B5*B9</f>
+        <v>1.893939393939394E-2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="1">
+        <f>B6*B10</f>
+        <v>0.12803030303030305</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP HV supply simulation
</commit_message>
<xml_diff>
--- a/KiCad/nixieAccurateClock/boost-convertor-calcs.xlsx
+++ b/KiCad/nixieAccurateClock/boost-convertor-calcs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Nextcloud\Documents\Projects\nixieclock\nixie-clock-ice\KiCad\nixieAccurateClock\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Nextcloud\Documents\Projects\nixieclock\nixie-clock-ice\KiCad\nixieAccurateClock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1929C828-BF49-40A9-B433-48AAA483BE00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E6B57B-A3E5-4CEB-B5B8-6BF94928A6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25560" yWindow="8310" windowWidth="23010" windowHeight="12360" xr2:uid="{4C5F7C1F-78F8-476C-9393-F25C88E783DB}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{4C5F7C1F-78F8-476C-9393-F25C88E783DB}"/>
   </bookViews>
   <sheets>
     <sheet name="HV supply" sheetId="1" r:id="rId1"/>
@@ -541,25 +541,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D3FE33C-00CB-4DD1-9E2D-595A71855D92}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7890625" customWidth="1"/>
+    <col min="2" max="2" width="11.5234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
         <v>20</v>
       </c>
@@ -570,7 +572,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -590,7 +592,7 @@
         <v>1.6799999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -607,7 +609,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -624,7 +626,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -644,7 +646,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -661,7 +663,7 @@
         <v>8.1999999999999998E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -681,7 +683,7 @@
         <v>1.5999999999999999E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -701,7 +703,7 @@
         <v>5.9523809523809521E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -718,7 +720,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -735,7 +737,7 @@
         <v>0.97619047619047616</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -755,7 +757,7 @@
         <v>7.0861678004535298E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -775,7 +777,7 @@
         <v>0.70559999999999923</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -795,7 +797,7 @@
         <v>0.735361904761904</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -842,12 +844,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.5234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -858,7 +860,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -869,7 +871,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -881,7 +883,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -893,7 +895,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -905,7 +907,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -917,7 +919,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -929,7 +931,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -941,7 +943,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -953,7 +955,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -965,7 +967,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
simulate HV supply concept
LM5156 simulation is infeasible

LTSpice model demonstrating that a two stage buck from 5 to 210 is possible.  Both stages run away, but the LM5156 should provide feedback to keep it on target.
</commit_message>
<xml_diff>
--- a/KiCad/nixieAccurateClock/boost-convertor-calcs.xlsx
+++ b/KiCad/nixieAccurateClock/boost-convertor-calcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Nextcloud\Documents\Projects\nixieclock\nixie-clock-ice\KiCad\nixieAccurateClock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7760DC-C0D9-420B-8C10-CD2A80A07D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CCE47A-4196-4F07-9339-C801DE5BCB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{4C5F7C1F-78F8-476C-9393-F25C88E783DB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>Calcs from Art of Electronics - 3rd Edition, Section 9.6.6.a Boost convertor equations (continuous-conduction mode)</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>20V</t>
   </si>
 </sst>
 </file>
@@ -188,7 +191,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -539,7 +582,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D3FE33C-00CB-4DD1-9E2D-595A71855D92}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -549,17 +592,17 @@
     <col min="2" max="2" width="11.5234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
         <v>20</v>
       </c>
@@ -569,8 +612,11 @@
       <c r="E3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="H3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -589,62 +635,76 @@
         <f>6*(2.5+0.3)*0.001</f>
         <v>1.6799999999999999E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="H5">
+        <f>6*(2.5+0.3)*0.001</f>
+        <v>1.6799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
       </c>
       <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="H6">
         <v>5</v>
       </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1">
-        <v>100000</v>
+        <v>47000</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="1">
-        <v>100000</v>
+        <v>47000</v>
       </c>
       <c r="E7" s="1">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>47000</v>
+      </c>
+      <c r="H7" s="1">
+        <v>219000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8">
         <f>1/B7</f>
-        <v>1.0000000000000001E-5</v>
+        <v>2.1276595744680852E-5</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
       </c>
       <c r="D8">
         <f>1/D7</f>
-        <v>1.0000000000000001E-5</v>
+        <v>2.1276595744680852E-5</v>
       </c>
       <c r="E8">
         <f>1/E7</f>
-        <v>1.0000000000000001E-5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>2.1276595744680852E-5</v>
+      </c>
+      <c r="H8">
+        <f>1/H7</f>
+        <v>4.5662100456621006E-6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -660,48 +720,59 @@
       <c r="E9" s="1">
         <v>8.1999999999999998E-4</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="H9" s="1">
+        <v>1.5E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>1</v>
       </c>
       <c r="B12">
         <f>B5/B14/B6</f>
-        <v>8.2352941176470581E-6</v>
+        <v>4.9411764705882345E-6</v>
       </c>
       <c r="C12" t="s">
         <v>15</v>
       </c>
       <c r="D12">
         <f>D5/D14/D6</f>
-        <v>2.2399999999999999E-5</v>
+        <v>6.999999999999999E-6</v>
       </c>
       <c r="E12">
         <f>E5/E14/E6</f>
-        <v>1.5999999999999999E-5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="H12">
+        <f>H5/H14/H6</f>
+        <v>1.6799999999999999E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13">
         <f>B8/B9*B6*B15</f>
-        <v>0.13601147776183647</v>
+        <v>0.45788943496443735</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
       </c>
       <c r="D13">
         <f>D8/D9*D6*D15</f>
-        <v>5.894308943089431E-2</v>
+        <v>0.43245113302196864</v>
       </c>
       <c r="E13">
         <f>E8/E9*E6*E15</f>
-        <v>5.9523809523809521E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>0.46951837299528021</v>
+      </c>
+      <c r="H13">
+        <f>H8/H9*H6*H15</f>
+        <v>1.1415525114155249</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -712,123 +783,154 @@
         <v>16</v>
       </c>
       <c r="D14">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="E14">
         <v>210</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="H14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="2">
         <f>1-(B6/B14)</f>
-        <v>0.92941176470588238</v>
+        <v>0.88235294117647056</v>
       </c>
       <c r="D15" s="2">
         <f>1-(D6/D14)</f>
-        <v>0.96666666666666667</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E15" s="2">
         <f>1-(E6/E14)</f>
-        <v>0.97619047619047616</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>0.90476190476190477</v>
+      </c>
+      <c r="H15" s="2">
+        <f>1-(H6/H14)</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>3</v>
       </c>
       <c r="B16">
         <f>B8/(2*B9)*B14*B15*POWER(1-B15,2)</f>
-        <v>4.8004050974765769E-3</v>
+        <v>2.693467264496691E-2</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
       </c>
       <c r="D16">
         <f>D8/(2*D9)*D14*D15*POWER(1-D15,2)</f>
-        <v>9.823848238482381E-4</v>
+        <v>3.6037594418497361E-2</v>
       </c>
       <c r="E16">
         <f>E8/(2*E9)*E14*E15*POWER(1-E15,2)</f>
-        <v>7.0861678004535298E-4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>2.2358017761680001E-2</v>
+      </c>
+      <c r="H16">
+        <f>H8/(2*H9)*H14*H15*POWER(1-H15,2)</f>
+        <v>0.14269406392694062</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>9</v>
       </c>
       <c r="B17">
         <f>B5/(1-B15)</f>
-        <v>0.23800000000000007</v>
+        <v>0.14279999999999995</v>
       </c>
       <c r="C17" t="s">
         <v>15</v>
       </c>
       <c r="D17">
         <f>D5/(1-D15)</f>
-        <v>0.50400000000000011</v>
+        <v>0.10080000000000001</v>
       </c>
       <c r="E17">
         <f>E5/(1-E15)</f>
-        <v>0.70559999999999923</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>0.1764</v>
+      </c>
+      <c r="H17">
+        <f>H5/(1-H15)</f>
+        <v>6.7199999999999996E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>4</v>
       </c>
       <c r="B18">
         <f>B5/(1-B15)+(B8/(2*B9)*B6*B15)</f>
-        <v>0.30600573888091831</v>
+        <v>0.3717447174822186</v>
       </c>
       <c r="C18" t="s">
         <v>15</v>
       </c>
       <c r="D18">
         <f>D5/(1-D15)+(D8/(2*D9)*D6*D15)</f>
-        <v>0.53347154471544722</v>
+        <v>0.31702556651098435</v>
       </c>
       <c r="E18">
         <f>E5/(1-E15)+(E8/(2*E9)*E6*E15)</f>
-        <v>0.735361904761904</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>0.41115918649764011</v>
+      </c>
+      <c r="H18">
+        <f>H5/(1-H15)+(H8/(2*H9)*H6*H15)</f>
+        <v>0.63797625570776251</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>5</v>
       </c>
       <c r="B19">
         <f>B8/(2*B5)*POWER(B6/B14,2)*(B14-B6)</f>
-        <v>2.3430548690064261E-4</v>
+        <v>1.3146685457662416E-3</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
       </c>
       <c r="D19">
         <f>D8/(2*D5)*POWER(D6/D14,2)*(D14-D6)</f>
-        <v>4.7949735449735452E-5</v>
+        <v>1.7589778228076101E-3</v>
       </c>
       <c r="E19">
         <f>E8/(2*E5)*POWER(E6/E14,2)*(E14-E6)</f>
-        <v>3.4587247597451676E-5</v>
+        <v>1.0912842002724764E-3</v>
+      </c>
+      <c r="H19">
+        <f>H8/(2*H5)*POWER(H6/H14,2)*(H14-H6)</f>
+        <v>1.2740541422048273E-4</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="lessThanOrEqual">
       <formula>$B$19</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThan">
       <formula>$B$19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:E9">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThanOrEqual">
       <formula>$B$19</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThan">
+      <formula>$B$19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThanOrEqual">
+      <formula>$B$19</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>$B$19</formula>
     </cfRule>
   </conditionalFormatting>
@@ -875,7 +977,7 @@
       </c>
       <c r="B4" s="1">
         <f>('HV supply'!D14-B1)/B3</f>
-        <v>1.5151515151515152E-4</v>
+        <v>-7.5757575757575758E-4</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -911,7 +1013,7 @@
       </c>
       <c r="B8" s="1">
         <f>B4*B3</f>
-        <v>5</v>
+        <v>-25</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
@@ -947,7 +1049,7 @@
       </c>
       <c r="B12" s="1">
         <f>B4*B8</f>
-        <v>7.5757575757575758E-4</v>
+        <v>1.893939393939394E-2</v>
       </c>
       <c r="C12" t="s">
         <v>35</v>

</xml_diff>